<commit_message>
#issue 1 : number case
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WindownFormApplication\WFA-GroupImages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF458E-937C-4ED9-80AF-1DF098351526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD40D2B-9EC8-4AB7-9284-D81D520AAE67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E448464-EBAB-4ACB-BB37-B78468DE8D2D}"/>
+    <workbookView xWindow="1005" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{8E448464-EBAB-4ACB-BB37-B78468DE8D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -739,21 +739,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2AF48C-0E32-4005-82B3-1B4DAB65A836}">
   <dimension ref="D3:X152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="K79" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P89" sqref="P89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="26.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="T3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>72</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>72</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>72</v>
       </c>
@@ -831,7 +831,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>72</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>72</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>72</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>72</v>
       </c>
@@ -935,7 +935,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>72</v>
       </c>
@@ -961,7 +961,7 @@
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>72</v>
       </c>
@@ -987,7 +987,7 @@
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>72</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>72</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>72</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>72</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>72</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>72</v>
       </c>
@@ -1143,7 +1143,7 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>72</v>
       </c>
@@ -1172,7 +1172,7 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>72</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>72</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>72</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>72</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>72</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>72</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>72</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>72</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>72</v>
       </c>
@@ -1435,7 +1435,7 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>72</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>72</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>72</v>
       </c>
@@ -1522,7 +1522,7 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>72</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
     </row>
-    <row r="34" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>72</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>72</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
     </row>
-    <row r="36" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>72</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>72</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>72</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>72</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
     </row>
-    <row r="40" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>72</v>
       </c>
@@ -1754,7 +1754,7 @@
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
     </row>
-    <row r="41" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>72</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>72</v>
       </c>
@@ -1812,7 +1812,7 @@
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>72</v>
       </c>
@@ -1841,7 +1841,7 @@
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
     </row>
-    <row r="44" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>72</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
     </row>
-    <row r="45" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>72</v>
       </c>
@@ -1899,7 +1899,7 @@
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
     </row>
-    <row r="46" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>72</v>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
     </row>
-    <row r="47" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>72</v>
       </c>
@@ -1957,7 +1957,7 @@
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
     </row>
-    <row r="48" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>72</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
     </row>
-    <row r="49" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>72</v>
       </c>
@@ -2015,7 +2015,7 @@
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
     </row>
-    <row r="50" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>72</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
     </row>
-    <row r="51" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>72</v>
       </c>
@@ -2073,7 +2073,7 @@
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
     </row>
-    <row r="52" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>72</v>
       </c>
@@ -2102,7 +2102,7 @@
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
     </row>
-    <row r="53" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>72</v>
       </c>
@@ -2131,7 +2131,7 @@
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
     </row>
-    <row r="54" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>72</v>
       </c>
@@ -2160,7 +2160,7 @@
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
     </row>
-    <row r="55" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>72</v>
       </c>
@@ -2189,7 +2189,7 @@
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
     </row>
-    <row r="56" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>72</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
     </row>
-    <row r="57" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>72</v>
       </c>
@@ -2247,7 +2247,7 @@
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
     </row>
-    <row r="58" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>72</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="W58" s="3"/>
       <c r="X58" s="3"/>
     </row>
-    <row r="59" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>72</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
     </row>
-    <row r="60" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>72</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="W60" s="3"/>
       <c r="X60" s="3"/>
     </row>
-    <row r="61" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>72</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="W61" s="3"/>
       <c r="X61" s="3"/>
     </row>
-    <row r="62" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2392,7 @@
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
     </row>
-    <row r="63" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>72</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
     </row>
-    <row r="64" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>72</v>
       </c>
@@ -2450,7 +2450,7 @@
       <c r="W64" s="3"/>
       <c r="X64" s="3"/>
     </row>
-    <row r="65" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>72</v>
       </c>
@@ -2479,7 +2479,7 @@
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
     </row>
-    <row r="66" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>72</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
     </row>
-    <row r="67" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>72</v>
       </c>
@@ -2537,7 +2537,7 @@
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>72</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="W68" s="3"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>72</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="W69" s="3"/>
       <c r="X69" s="3"/>
     </row>
-    <row r="70" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>72</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>72</v>
       </c>
@@ -2653,7 +2653,7 @@
       <c r="W71" s="3"/>
       <c r="X71" s="3"/>
     </row>
-    <row r="72" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>72</v>
       </c>
@@ -2682,7 +2682,7 @@
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
     </row>
-    <row r="73" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>72</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="W73" s="3"/>
       <c r="X73" s="3"/>
     </row>
-    <row r="74" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>72</v>
       </c>
@@ -2740,7 +2740,7 @@
       <c r="W74" s="3"/>
       <c r="X74" s="3"/>
     </row>
-    <row r="75" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:24" x14ac:dyDescent="0.25">
       <c r="P75" s="3" t="s">
         <v>60</v>
       </c>
@@ -2753,7 +2753,7 @@
       <c r="W75" s="3"/>
       <c r="X75" s="3"/>
     </row>
-    <row r="78" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:24" x14ac:dyDescent="0.25">
       <c r="P78" s="7" t="s">
         <v>43</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:24" x14ac:dyDescent="0.25">
       <c r="P79" s="7" t="s">
         <v>34</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="S79" s="7"/>
       <c r="T79" s="7"/>
     </row>
-    <row r="80" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:24" x14ac:dyDescent="0.25">
       <c r="P80" s="7" t="s">
         <v>22</v>
       </c>
@@ -2783,7 +2783,7 @@
       <c r="S80" s="7"/>
       <c r="T80" s="7"/>
     </row>
-    <row r="81" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:24" x14ac:dyDescent="0.25">
       <c r="P81" s="7" t="s">
         <v>23</v>
       </c>
@@ -2792,7 +2792,7 @@
       <c r="S81" s="7"/>
       <c r="T81" s="7"/>
     </row>
-    <row r="82" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>11</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="S82" s="7"/>
       <c r="T82" s="7"/>
     </row>
-    <row r="83" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:24" x14ac:dyDescent="0.25">
       <c r="P83" s="7" t="s">
         <v>12</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="S83" s="7"/>
       <c r="T83" s="7"/>
     </row>
-    <row r="84" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>74</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="S84" s="7"/>
       <c r="T84" s="7"/>
     </row>
-    <row r="85" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
         <v>77</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="S85" s="7"/>
       <c r="T85" s="7"/>
     </row>
-    <row r="86" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
         <v>79</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
         <v>22</v>
       </c>
@@ -2877,7 +2877,7 @@
       <c r="W88" s="4"/>
       <c r="X88" s="4"/>
     </row>
-    <row r="89" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
         <v>74</v>
       </c>
@@ -2899,7 +2899,7 @@
       <c r="W89" s="4"/>
       <c r="X89" s="4"/>
     </row>
-    <row r="90" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
         <v>77</v>
       </c>
@@ -2922,7 +2922,7 @@
       <c r="W90" s="4"/>
       <c r="X90" s="4"/>
     </row>
-    <row r="91" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F91" t="s">
         <v>79</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="W91" s="4"/>
       <c r="X91" s="4"/>
     </row>
-    <row r="92" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:24" x14ac:dyDescent="0.25">
       <c r="P92" s="4" t="s">
         <v>6</v>
       </c>
@@ -2957,7 +2957,7 @@
       <c r="W92" s="4"/>
       <c r="X92" s="4"/>
     </row>
-    <row r="93" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
         <v>86</v>
       </c>
@@ -2973,7 +2973,7 @@
       <c r="W93" s="4"/>
       <c r="X93" s="4"/>
     </row>
-    <row r="94" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
         <v>87</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="W94" s="4"/>
       <c r="X94" s="4"/>
     </row>
-    <row r="95" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:24" x14ac:dyDescent="0.25">
       <c r="P95" s="4" t="s">
         <v>8</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="W95" s="4"/>
       <c r="X95" s="4"/>
     </row>
-    <row r="96" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:24" x14ac:dyDescent="0.25">
       <c r="P96" s="4" t="s">
         <v>30</v>
       </c>
@@ -3015,7 +3015,7 @@
       <c r="W96" s="4"/>
       <c r="X96" s="4"/>
     </row>
-    <row r="97" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="97" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P97" s="4" t="s">
         <v>58</v>
       </c>
@@ -3028,7 +3028,7 @@
       <c r="W97" s="4"/>
       <c r="X97" s="4"/>
     </row>
-    <row r="98" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="98" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P98" s="7" t="s">
         <v>62</v>
       </c>
@@ -3041,7 +3041,7 @@
       <c r="W98" s="4"/>
       <c r="X98" s="4"/>
     </row>
-    <row r="99" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="99" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P99" s="4" t="s">
         <v>35</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="W99" s="4"/>
       <c r="X99" s="4"/>
     </row>
-    <row r="100" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="100" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P100" s="4" t="s">
         <v>53</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="W100" s="4"/>
       <c r="X100" s="4"/>
     </row>
-    <row r="101" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="101" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P101" s="7" t="s">
         <v>59</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="W101" s="4"/>
       <c r="X101" s="4"/>
     </row>
-    <row r="102" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="102" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P102" s="4" t="s">
         <v>36</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="W102" s="4"/>
       <c r="X102" s="4"/>
     </row>
-    <row r="103" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="103" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P103" s="4" t="s">
         <v>26</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="W103" s="4"/>
       <c r="X103" s="4"/>
     </row>
-    <row r="104" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="104" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P104" s="4" t="s">
         <v>25</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="W104" s="4"/>
       <c r="X104" s="4"/>
     </row>
-    <row r="105" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="105" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P105" s="4" t="s">
         <v>20</v>
       </c>
@@ -3134,7 +3134,7 @@
       <c r="W105" s="4"/>
       <c r="X105" s="4"/>
     </row>
-    <row r="106" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="106" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P106" s="4" t="s">
         <v>9</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="W106" s="4"/>
       <c r="X106" s="4"/>
     </row>
-    <row r="107" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="107" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P107" s="4" t="s">
         <v>69</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="W107" s="4"/>
       <c r="X107" s="4"/>
     </row>
-    <row r="108" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="108" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P108" s="4" t="s">
         <v>44</v>
       </c>
@@ -3173,7 +3173,7 @@
       <c r="W108" s="4"/>
       <c r="X108" s="4"/>
     </row>
-    <row r="109" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="109" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P109" s="4" t="s">
         <v>2</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="W109" s="4"/>
       <c r="X109" s="4"/>
     </row>
-    <row r="110" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="110" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P110" s="4" t="s">
         <v>21</v>
       </c>
@@ -3199,7 +3199,7 @@
       <c r="W110" s="4"/>
       <c r="X110" s="4"/>
     </row>
-    <row r="111" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="111" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P111" s="4" t="s">
         <v>67</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="W111" s="4"/>
       <c r="X111" s="4"/>
     </row>
-    <row r="112" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="112" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P112" s="4" t="s">
         <v>10</v>
       </c>
@@ -3225,7 +3225,7 @@
       <c r="W112" s="4"/>
       <c r="X112" s="4"/>
     </row>
-    <row r="113" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="113" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P113" s="4" t="s">
         <v>27</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="W113" s="4"/>
       <c r="X113" s="4"/>
     </row>
-    <row r="114" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="114" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P114" s="4" t="s">
         <v>64</v>
       </c>
@@ -3251,7 +3251,7 @@
       <c r="W114" s="4"/>
       <c r="X114" s="4"/>
     </row>
-    <row r="115" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="115" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P115" s="4" t="s">
         <v>0</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="W115" s="4"/>
       <c r="X115" s="4"/>
     </row>
-    <row r="116" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="116" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P116" s="4" t="s">
         <v>29</v>
       </c>
@@ -3277,7 +3277,7 @@
       <c r="W116" s="4"/>
       <c r="X116" s="4"/>
     </row>
-    <row r="117" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="117" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P117" s="4" t="s">
         <v>65</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="W117" s="4"/>
       <c r="X117" s="4"/>
     </row>
-    <row r="118" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="118" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P118" s="7" t="s">
         <v>66</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="W118" s="4"/>
       <c r="X118" s="4"/>
     </row>
-    <row r="119" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="119" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P119" s="4" t="s">
         <v>37</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="W119" s="4"/>
       <c r="X119" s="4"/>
     </row>
-    <row r="120" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="120" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P120" s="4" t="s">
         <v>47</v>
       </c>
@@ -3329,7 +3329,7 @@
       <c r="W120" s="4"/>
       <c r="X120" s="4"/>
     </row>
-    <row r="121" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="121" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P121" s="7" t="s">
         <v>57</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="W121" s="4"/>
       <c r="X121" s="4"/>
     </row>
-    <row r="122" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="122" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P122" s="4" t="s">
         <v>68</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="W122" s="4"/>
       <c r="X122" s="4"/>
     </row>
-    <row r="123" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="123" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P123" s="4" t="s">
         <v>49</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="W123" s="4"/>
       <c r="X123" s="4"/>
     </row>
-    <row r="124" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="124" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P124" s="4" t="s">
         <v>16</v>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="W124" s="4"/>
       <c r="X124" s="4"/>
     </row>
-    <row r="125" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="125" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P125" s="4" t="s">
         <v>45</v>
       </c>
@@ -3394,7 +3394,7 @@
       <c r="W125" s="4"/>
       <c r="X125" s="4"/>
     </row>
-    <row r="126" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="126" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P126" s="4" t="s">
         <v>17</v>
       </c>
@@ -3407,7 +3407,7 @@
       <c r="W126" s="4"/>
       <c r="X126" s="4"/>
     </row>
-    <row r="127" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="127" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P127" s="7" t="s">
         <v>63</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="W127" s="4"/>
       <c r="X127" s="4"/>
     </row>
-    <row r="128" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="128" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P128" s="4" t="s">
         <v>56</v>
       </c>
@@ -3433,7 +3433,7 @@
       <c r="W128" s="4"/>
       <c r="X128" s="4"/>
     </row>
-    <row r="131" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P131" s="5" t="s">
         <v>3</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="T131" s="5"/>
       <c r="U131" s="5"/>
     </row>
-    <row r="132" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P132" s="5" t="s">
         <v>4</v>
       </c>
@@ -3453,7 +3453,7 @@
       <c r="T132" s="5"/>
       <c r="U132" s="5"/>
     </row>
-    <row r="133" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P133" s="5" t="s">
         <v>31</v>
       </c>
@@ -3463,7 +3463,7 @@
       <c r="T133" s="5"/>
       <c r="U133" s="5"/>
     </row>
-    <row r="134" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="134" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P134" s="5" t="s">
         <v>38</v>
       </c>
@@ -3473,7 +3473,7 @@
       <c r="T134" s="5"/>
       <c r="U134" s="5"/>
     </row>
-    <row r="135" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P135" s="5" t="s">
         <v>33</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="T135" s="5"/>
       <c r="U135" s="5"/>
     </row>
-    <row r="136" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P136" s="5" t="s">
         <v>52</v>
       </c>
@@ -3493,7 +3493,7 @@
       <c r="T136" s="5"/>
       <c r="U136" s="5"/>
     </row>
-    <row r="137" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P137" s="5" t="s">
         <v>18</v>
       </c>
@@ -3503,7 +3503,7 @@
       <c r="T137" s="5"/>
       <c r="U137" s="5"/>
     </row>
-    <row r="138" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="138" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P138" s="5" t="s">
         <v>7</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="T138" s="5"/>
       <c r="U138" s="5"/>
     </row>
-    <row r="139" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P139" s="5" t="s">
         <v>42</v>
       </c>
@@ -3523,7 +3523,7 @@
       <c r="T139" s="5"/>
       <c r="U139" s="5"/>
     </row>
-    <row r="140" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P140" s="5" t="s">
         <v>14</v>
       </c>
@@ -3533,7 +3533,7 @@
       <c r="T140" s="5"/>
       <c r="U140" s="5"/>
     </row>
-    <row r="141" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P141" s="5" t="s">
         <v>60</v>
       </c>
@@ -3543,7 +3543,7 @@
       <c r="T141" s="5"/>
       <c r="U141" s="5"/>
     </row>
-    <row r="144" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="144" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P144" s="6" t="s">
         <v>39</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="T144" s="6"/>
       <c r="U144" s="6"/>
     </row>
-    <row r="145" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="145" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P145" s="6" t="s">
         <v>40</v>
       </c>
@@ -3563,7 +3563,7 @@
       <c r="T145" s="6"/>
       <c r="U145" s="6"/>
     </row>
-    <row r="146" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="146" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P146" s="6" t="s">
         <v>54</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="T146" s="6"/>
       <c r="U146" s="6"/>
     </row>
-    <row r="147" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="147" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P147" s="6" t="s">
         <v>48</v>
       </c>
@@ -3583,7 +3583,7 @@
       <c r="T147" s="6"/>
       <c r="U147" s="6"/>
     </row>
-    <row r="148" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="148" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P148" s="6" t="s">
         <v>46</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
     </row>
-    <row r="149" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="149" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P149" s="6" t="s">
         <v>50</v>
       </c>
@@ -3603,7 +3603,7 @@
       <c r="T149" s="6"/>
       <c r="U149" s="6"/>
     </row>
-    <row r="150" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="150" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P150" s="6" t="s">
         <v>41</v>
       </c>
@@ -3613,7 +3613,7 @@
       <c r="T150" s="6"/>
       <c r="U150" s="6"/>
     </row>
-    <row r="151" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="151" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P151" s="6" t="s">
         <v>51</v>
       </c>
@@ -3623,7 +3623,7 @@
       <c r="T151" s="6"/>
       <c r="U151" s="6"/>
     </row>
-    <row r="152" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="152" spans="16:21" x14ac:dyDescent="0.25">
       <c r="P152" s="6" t="s">
         <v>55</v>
       </c>

</xml_diff>